<commit_message>
write csv - first test
</commit_message>
<xml_diff>
--- a/operationFolder/downloads/data_excel.xlsx
+++ b/operationFolder/downloads/data_excel.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="General" sheetId="2" r:id="rId1"/>
-    <sheet name="test2" sheetId="1" r:id="rId2"/>
-    <sheet name="test3" sheetId="3" r:id="rId3"/>
+    <sheet name="Normal" sheetId="2" r:id="rId1"/>
+    <sheet name="WithNewLine" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="60">
   <si>
     <t>Decimal</t>
   </si>
@@ -173,32 +172,35 @@
     <t>BT-LAH-21</t>
   </si>
   <si>
-    <t>AU40x Audi A4AU436
+    <t>Confidential.</t>
+  </si>
+  <si>
+    <t>If the contractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the contractor discovers </t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>This BT-LAH</t>
+  </si>
+  <si>
+    <t>The present component specification and the standard VW 99000 incl</t>
+  </si>
+  <si>
+    <t>VDA</t>
+  </si>
+  <si>
+    <t>The requirements</t>
+  </si>
+  <si>
+    <t>AU40x Audi A4AU436 Audi Q5</t>
+  </si>
+  <si>
+    <t>AU40x Audi A4AU436 
 Audi Q5</t>
-  </si>
-  <si>
-    <t>Confidential.</t>
-  </si>
-  <si>
-    <t>If the contractor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the contractor discovers </t>
-  </si>
-  <si>
-    <t>The</t>
-  </si>
-  <si>
-    <t>This BT-LAH</t>
-  </si>
-  <si>
-    <t>The present component specification and the standard VW 99000 incl</t>
-  </si>
-  <si>
-    <t>VDA</t>
-  </si>
-  <si>
-    <t>The requirements</t>
   </si>
 </sst>
 </file>
@@ -658,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,7 +722,7 @@
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>10</v>
@@ -737,7 +739,7 @@
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>12</v>
@@ -771,7 +773,7 @@
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>15</v>
@@ -788,7 +790,7 @@
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>17</v>
@@ -924,7 +926,7 @@
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>32</v>
@@ -941,7 +943,7 @@
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>33</v>
@@ -958,7 +960,7 @@
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>34</v>
@@ -992,7 +994,7 @@
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>37</v>
@@ -1096,7 +1098,7 @@
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>49</v>
@@ -1113,28 +1115,457 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.90625" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write csv - first test/end
</commit_message>
<xml_diff>
--- a/operationFolder/downloads/data_excel.xlsx
+++ b/operationFolder/downloads/data_excel.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="Normal" sheetId="2" r:id="rId1"/>
-    <sheet name="WithNewLine" sheetId="1" r:id="rId2"/>
+    <sheet name="CalcNr" sheetId="6" r:id="rId1"/>
+    <sheet name="Normal" sheetId="2" r:id="rId2"/>
+    <sheet name="WithNewN" sheetId="1" r:id="rId3"/>
+    <sheet name="WithNewLine" sheetId="3" r:id="rId4"/>
+    <sheet name="WithNewLineWithNr" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="65">
   <si>
     <t>Decimal</t>
   </si>
@@ -201,13 +204,28 @@
   <si>
     <t>AU40x Audi A4AU436 
 Audi Q5</t>
+  </si>
+  <si>
+    <t>Dec To Hex</t>
+  </si>
+  <si>
+    <t>Dec To Bin</t>
+  </si>
+  <si>
+    <t>Inverted (Dec To Hex)</t>
+  </si>
+  <si>
+    <t>Inverted (Dec To Bin)</t>
+  </si>
+  <si>
+    <t>Nr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +258,14 @@
     <font>
       <b/>
       <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -342,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -376,6 +402,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -658,10 +694,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>25966</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1234</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>975</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>543456</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>57886</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>223466</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>33467</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>21137</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
+        <v>44</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12">
+        <v>657</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12">
+        <v>941</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12">
+        <v>3468</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12">
+        <v>7521</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12">
+        <v>345676</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12">
+        <v>345</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12">
+        <v>6589</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12">
+        <v>9879</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="12">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12">
+        <v>23</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12">
+        <v>546</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="12">
+        <v>22</v>
+      </c>
+      <c r="B23" s="12">
+        <v>56567</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12">
+        <v>324</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12">
+        <v>24</v>
+      </c>
+      <c r="B25" s="12">
+        <v>7899</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1113,12 +1480,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1568,4 +1935,938 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.90625" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
+        <v>24</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.90625" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>25</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
+        <v>24</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>